<commit_message>
Adding conclusion into results
</commit_message>
<xml_diff>
--- a/machine_learning/CNN/results/FinalResults.xlsx
+++ b/machine_learning/CNN/results/FinalResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo22\Documents\ENSICAEN\Stage à l'étranger\Projet\lying-pen-scribes-project\machine_learning\CNN\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8CC608-D24C-4335-9C85-F7DB6578532C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8A65CB-9754-4708-9FFC-CBF37764DA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{98236539-3DA2-4643-A8C0-4B3CF68E3E49}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Nb Epochs</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>Batch Size</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>As we can see from these results, applying an early stopping criteria that is much more relevant to the current context has enabled us to achieve satisfactory accuracy (above 94%) while avoiding overlearning. Applying an optimiser with momentum and weight decay has a positive influence on the final results and on gradient descent during training.</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -253,6 +259,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C3A29D-D681-4FEF-AC54-721C190649E5}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -949,7 +958,37 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>